<commit_message>
update final main contribution
</commit_message>
<xml_diff>
--- a/content/species/data/Expert list for NBA.xlsx
+++ b/content/species/data/Expert list for NBA.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Maphale Monyeki Projects\NBA 2025\2. NBA 2025 - Modules\2. Modules\species\quarto\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_repos\species\quarto\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95432CF6-7242-417D-8A8E-09ED34FB6FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D5532B-2FC5-4922-9450-E9C3F9D754F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C5F6DE13-3553-4A3B-BACE-C3ADC42B365C}"/>
+    <workbookView xWindow="36150" yWindow="3150" windowWidth="17280" windowHeight="12330" xr2:uid="{C5F6DE13-3553-4A3B-BACE-C3ADC42B365C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$167</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$168</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="272">
   <si>
     <t>Affiliation</t>
   </si>
@@ -875,6 +875,9 @@
   </si>
   <si>
     <t>Esethu Nkibi</t>
+  </si>
+  <si>
+    <t>Carol Poole</t>
   </si>
 </sst>
 </file>
@@ -1305,10 +1308,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6E5F385-F8A0-44ED-A641-299CF61FE94C}">
-  <dimension ref="A1:B167"/>
+  <dimension ref="A1:B168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1454,384 +1457,384 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>30</v>
+      <c r="A18" s="3" t="s">
+        <v>271</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
+    <row r="28" spans="1:2" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>70</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>270</v>
+        <v>73</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>74</v>
+        <v>270</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>76</v>
+        <v>27</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>4</v>
+        <v>81</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>84</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>13</v>
+        <v>88</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>91</v>
+        <v>13</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>13</v>
+        <v>99</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>102</v>
+        <v>13</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B61" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="6" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B62" s="2" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>109</v>
+        <v>13</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>13</v>
+        <v>109</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>13</v>
@@ -1839,231 +1842,231 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>113</v>
+        <v>13</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B70" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" s="5" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>63</v>
+        <v>124</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>127</v>
+        <v>63</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" s="5" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B79" s="2" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>27</v>
+        <v>135</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>138</v>
+        <v>27</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>45</v>
+        <v>138</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>141</v>
+        <v>45</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>63</v>
+        <v>145</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>148</v>
+        <v>63</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>122</v>
+        <v>150</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>6</v>
+        <v>122</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>4</v>
@@ -2071,215 +2074,215 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>88</v>
+        <v>4</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>159</v>
+        <v>88</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>33</v>
+        <v>165</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>168</v>
+        <v>33</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>27</v>
+        <v>168</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>70</v>
+        <v>27</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>4</v>
+        <v>70</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B105" s="2" t="s">
+      <c r="B106" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A106" s="5" t="s">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="B107" s="2" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A107" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>176</v>
+        <v>88</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>99</v>
+        <v>178</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>181</v>
+        <v>99</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>76</v>
+        <v>181</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>186</v>
+        <v>4</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>43</v>
+        <v>188</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>4</v>
@@ -2287,175 +2290,175 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B122" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
+      </c>
+      <c r="B123" s="4" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>27</v>
+        <v>197</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>200</v>
+        <v>27</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>8</v>
+        <v>204</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B130" s="2" t="s">
+      <c r="B131" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A131" s="5" t="s">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="B131" s="2" t="s">
+      <c r="B132" s="2" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A132" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="B132" s="2" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>45</v>
+        <v>213</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="B135" s="2" t="s">
+      <c r="B136" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A136" s="5" t="s">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A137" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="B136" s="2" t="s">
+      <c r="B137" s="2" t="s">
         <v>217</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A137" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>27</v>
+        <v>227</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B143" s="2" t="s">
         <v>27</v>
@@ -2463,87 +2466,87 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>268</v>
+        <v>27</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A146" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="B145" s="2" t="s">
+      <c r="B146" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A146" s="6" t="s">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A147" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="B146" s="2" t="s">
+      <c r="B147" s="2" t="s">
         <v>233</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A147" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="B147" s="2" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>4</v>
+        <v>235</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>93</v>
+        <v>4</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>239</v>
+        <v>93</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>113</v>
+        <v>239</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>242</v>
+        <v>113</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>25</v>
+        <v>242</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B154" s="2" t="s">
         <v>25</v>
@@ -2551,112 +2554,120 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>246</v>
+        <v>25</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A157" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="B156" s="2" t="s">
+      <c r="B157" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A157" s="3" t="s">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A158" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="B157" s="2" t="s">
+      <c r="B158" s="2" t="s">
         <v>249</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A158" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="B158" s="2" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>99</v>
+        <v>251</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>254</v>
+        <v>99</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A162" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="B161" s="2" t="s">
+      <c r="B162" s="2" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A162" s="3" t="s">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A163" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="B162" s="2" t="s">
+      <c r="B163" s="2" t="s">
         <v>258</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A163" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="B163" s="2" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A165" s="2" t="s">
         <v>261</v>
-      </c>
-      <c r="B164" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A165" s="5" t="s">
-        <v>262</v>
       </c>
       <c r="B165" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A166" s="2" t="s">
-        <v>263</v>
+      <c r="A166" s="5" t="s">
+        <v>262</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>264</v>
+        <v>15</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A168" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="B167" s="2" t="s">
+      <c r="B168" s="2" t="s">
         <v>266</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B167" xr:uid="{C6E5F385-F8A0-44ED-A641-299CF61FE94C}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B167">
-      <sortCondition ref="A1:A167"/>
+  <autoFilter ref="A1:B168" xr:uid="{C6E5F385-F8A0-44ED-A641-299CF61FE94C}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B168">
+      <sortCondition ref="A1:A168"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2677,6 +2688,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A9251B87A2689245AA9FD86C69F20C58" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c860c8d8cea428af55d2deb18db3c3b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="de6781d5-cbdf-44cc-b8b1-919d4413b058" xmlns:ns3="d08e37f2-beba-4595-a3e8-aa91f032b3fc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a1915556badb0c1501ee51a52d85f263" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2954,15 +2974,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96CDBF78-4A9E-452E-AF29-C947CA5C59AF}">
   <ds:schemaRefs>
@@ -2976,6 +2987,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{567247E4-1E5D-466C-A424-05E84918D559}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5BEBDFE-E2C9-4275-B6D7-FDA513885B71}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2993,12 +3012,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{567247E4-1E5D-466C-A424-05E84918D559}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>